<commit_message>
Fix redundant code in report.php, fix insertion of series.
</commit_message>
<xml_diff>
--- a/Overall Report.xlsx
+++ b/Overall Report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
   <si>
     <t>Overall Report</t>
   </si>
@@ -41,7 +41,7 @@
     <t>Status / Accountability</t>
   </si>
   <si>
-    <t>AVR, Secure, , FFE- COMP-BCD-1297</t>
+    <t>4 GB RAM PC3 12800, , , 740617140743</t>
   </si>
   <si>
     <t>Furniture, Fixtures and Equipment</t>
@@ -50,70 +50,10 @@
     <t>Computer Equipment</t>
   </si>
   <si>
-    <t>Shoppers Guide</t>
-  </si>
-  <si>
-    <t>Ladi Joy Bacong</t>
-  </si>
-  <si>
-    <t>AVR, Secure, , FFE- COMP-BCD-1313</t>
-  </si>
-  <si>
-    <t>Renewable Energy Department</t>
-  </si>
-  <si>
-    <t>Alma Lucerna</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AVR, , , </t>
-  </si>
-  <si>
-    <t>Available</t>
-  </si>
-  <si>
-    <t>AVR, Secure, , IT20190321</t>
-  </si>
-  <si>
-    <t>Accounting</t>
-  </si>
-  <si>
-    <t>Damaged</t>
-  </si>
-  <si>
-    <t>Trading Department</t>
-  </si>
-  <si>
-    <t>Heziel Aplaon</t>
-  </si>
-  <si>
-    <t>AVR, Secure, , FFE- COMP-BCD-1348</t>
-  </si>
-  <si>
-    <t>AVR, Secure, , FFE- COMP-BCD-1362</t>
-  </si>
-  <si>
-    <t>Contracts &amp; Compliance</t>
-  </si>
-  <si>
-    <t>Teresa Tan</t>
-  </si>
-  <si>
-    <t>AVR, , , FFE- COMP-BCD-1367</t>
-  </si>
-  <si>
-    <t>HR/Admin</t>
-  </si>
-  <si>
-    <t>Babylyn C. Providencia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AVR , Secure Standard, , </t>
-  </si>
-  <si>
-    <t>Engineering/ Renewable Energy</t>
-  </si>
-  <si>
-    <t>Ana Marie Mangubat</t>
+    <t>EMG-Billing</t>
+  </si>
+  <si>
+    <t>Celina Marie Grabillo</t>
   </si>
 </sst>
 </file>
@@ -499,7 +439,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -507,13 +447,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="39.990234" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="43.560791" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="5.855713" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="8.140869" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="5.855713" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="39.990234" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="22.280273" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="35.2771" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="26.993408" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="13.996582" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="25.85083" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -570,248 +510,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="2">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="2">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2">
-        <v>240</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="2">
-        <v>1</v>
-      </c>
-      <c r="C6" s="2">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="2">
-        <v>1</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="2">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="2">
-        <v>1</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="2">
-        <v>1</v>
-      </c>
-      <c r="C10" s="2">
-        <v>240</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="2">
-        <v>1</v>
-      </c>
-      <c r="C11" s="2">
-        <v>0</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="2">
-        <v>1</v>
-      </c>
-      <c r="C12" s="2">
-        <v>0</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="2">
-        <v>1</v>
-      </c>
-      <c r="C13" s="2">
-        <v>240</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
   </sheetData>
   <sheetProtection sheet="true" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <protectedRanges>
     <protectedRange name="p72c8ec415e21b0ae7640bf770ec725aa" sqref="A3:G3" password="C724"/>
-    <protectedRange name="p6804d5b44d5f0d4113024046398c096e" sqref="A4:G4" password="C724"/>
-    <protectedRange name="pc8420570319781b040e4fc77750462f7" sqref="A5:G5" password="C724"/>
-    <protectedRange name="p8d708506dfc8ef2b51c8cf4c5cc3f33e" sqref="A6:G6" password="C724"/>
-    <protectedRange name="p7e546d096378a890fc57fdb0eb79006b" sqref="A7:G7" password="C724"/>
-    <protectedRange name="p41ea1506cf0897ae247c4f5c88018854" sqref="A8:G8" password="C724"/>
-    <protectedRange name="pb50b084456ae1386075f58d9fe331648" sqref="A9:G9" password="C724"/>
-    <protectedRange name="p104b3f0827a65187bcaf8c19e19d8450" sqref="A10:G10" password="C724"/>
-    <protectedRange name="pbbed5f6e5fdf4ff6b71bd6209e3a80cc" sqref="A11:G11" password="C724"/>
-    <protectedRange name="p4dd2f9099d40a8de727a847709c3a2b4" sqref="A12:G12" password="C724"/>
-    <protectedRange name="p7da544e962e0ee3a2fcd81e0a9e771e0" sqref="A13:G13" password="C724"/>
   </protectedRanges>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>